<commit_message>
New improvement + kuantitatif(masih error)
</commit_message>
<xml_diff>
--- a/assets/upload/Kuantitatif.xlsx
+++ b/assets/upload/Kuantitatif.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="154">
   <si>
     <t>Nomor Inisiatif</t>
   </si>
@@ -806,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -881,8 +881,8 @@
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
+      <c r="D4" s="1">
+        <v>0</v>
       </c>
       <c r="E4" s="1">
         <v>10</v>

</xml_diff>